<commit_message>
Update app.py with new form fields
</commit_message>
<xml_diff>
--- a/国内移動届.xlsx
+++ b/国内移動届.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="121">
   <si>
     <t>【移動届】出張・旅行申請フォーマット</t>
   </si>
@@ -275,9 +275,6 @@
       </rPr>
       <t>：</t>
     </r>
-  </si>
-  <si>
-    <t>Field Trip</t>
   </si>
   <si>
     <r>
@@ -3780,9 +3777,7 @@
         <v>37</v>
       </c>
       <c r="B24" s="46"/>
-      <c r="C24" s="59" t="s">
-        <v>38</v>
-      </c>
+      <c r="C24" s="59"/>
       <c r="D24" s="48"/>
       <c r="E24" s="48"/>
       <c r="F24" s="48"/>
@@ -3809,7 +3804,7 @@
     </row>
     <row r="25" ht="28.5" customHeight="1">
       <c r="A25" s="46" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B25" s="46"/>
       <c r="C25" s="60"/>
@@ -3839,12 +3834,12 @@
     </row>
     <row r="26" ht="28.5" customHeight="1">
       <c r="A26" s="46" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26" s="46"/>
       <c r="C26" s="62"/>
       <c r="D26" s="63" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E26" s="62"/>
       <c r="F26" s="45"/>
@@ -3871,11 +3866,11 @@
     </row>
     <row r="27" ht="28.5" customHeight="1">
       <c r="A27" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B27" s="19"/>
       <c r="C27" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D27" s="64">
         <v>1.0</v>
@@ -3906,17 +3901,17 @@
     <row r="28" ht="28.5" customHeight="1">
       <c r="A28" s="65"/>
       <c r="B28" s="66" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C28" s="67" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D28" s="65"/>
       <c r="E28" s="68" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F28" s="67" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G28" s="19"/>
       <c r="H28" s="19"/>
@@ -3944,10 +3939,10 @@
         <v>1.0</v>
       </c>
       <c r="B29" s="70" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C29" s="71" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D29" s="72">
         <v>6.0</v>
@@ -4105,20 +4100,20 @@
     </row>
     <row r="34" ht="28.5" customHeight="1">
       <c r="A34" s="81" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B34" s="82"/>
       <c r="C34" s="83"/>
       <c r="D34" s="84"/>
       <c r="E34" s="35" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F34" s="85">
         <v>2.54704387792E11</v>
       </c>
       <c r="G34" s="48"/>
       <c r="H34" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I34" s="19"/>
       <c r="J34" s="19"/>
@@ -4169,7 +4164,7 @@
     </row>
     <row r="36" ht="39.75" customHeight="1">
       <c r="A36" s="46" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B36" s="19"/>
       <c r="C36" s="88"/>
@@ -4199,33 +4194,33 @@
     </row>
     <row r="37" ht="39.75" customHeight="1">
       <c r="A37" s="89" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B37" s="90" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="90" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="91" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G37" s="90" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H37" s="24"/>
       <c r="I37" s="24"/>
       <c r="J37" s="4"/>
       <c r="K37" s="90" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L37" s="24"/>
       <c r="M37" s="24"/>
       <c r="N37" s="4"/>
       <c r="O37" s="90" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="P37" s="24"/>
       <c r="Q37" s="24"/>
@@ -4242,44 +4237,44 @@
     <row r="38" ht="39.75" customHeight="1">
       <c r="A38" s="6"/>
       <c r="B38" s="92" t="s">
+        <v>58</v>
+      </c>
+      <c r="C38" s="93" t="s">
         <v>59</v>
       </c>
-      <c r="C38" s="93" t="s">
-        <v>60</v>
-      </c>
       <c r="D38" s="92" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E38" s="93" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F38" s="6"/>
       <c r="G38" s="92" t="s">
+        <v>60</v>
+      </c>
+      <c r="H38" s="94" t="s">
         <v>61</v>
       </c>
-      <c r="H38" s="94" t="s">
+      <c r="I38" s="94" t="s">
         <v>62</v>
       </c>
-      <c r="I38" s="94" t="s">
+      <c r="J38" s="94" t="s">
         <v>63</v>
       </c>
-      <c r="J38" s="94" t="s">
+      <c r="K38" s="95" t="s">
         <v>64</v>
-      </c>
-      <c r="K38" s="95" t="s">
-        <v>65</v>
       </c>
       <c r="L38" s="96"/>
       <c r="M38" s="97" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N38" s="4"/>
       <c r="O38" s="90" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P38" s="4"/>
       <c r="Q38" s="90" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="R38" s="4"/>
       <c r="S38" s="88"/>
@@ -4646,7 +4641,7 @@
       <c r="P51" s="19"/>
       <c r="Q51" s="19"/>
       <c r="R51" s="35" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="S51" s="20"/>
       <c r="T51" s="20"/>
@@ -31343,12 +31338,12 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="144" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="145" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" s="146">
         <f>COUNTA(A2:A6)</f>
@@ -31357,258 +31352,258 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="145" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25" customHeight="1">
+      <c r="A4" s="145" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="145" t="s">
+    <row r="5" ht="14.25" customHeight="1">
+      <c r="A5" s="145" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="145" t="s">
+    <row r="6" ht="14.25" customHeight="1">
+      <c r="A6" s="145" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="145" t="s">
+    <row r="7" ht="14.25" customHeight="1">
+      <c r="A7" s="145" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="145" t="s">
+    <row r="8" ht="14.25" customHeight="1">
+      <c r="A8" s="145" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="145" t="s">
+    <row r="9" ht="14.25" customHeight="1">
+      <c r="A9" s="145" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" s="145" t="s">
+    <row r="10" ht="14.25" customHeight="1">
+      <c r="A10" s="145" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="10" ht="14.25" customHeight="1">
-      <c r="A10" s="145" t="s">
+      <c r="B10" s="147"/>
+    </row>
+    <row r="11" ht="14.25" customHeight="1">
+      <c r="A11" s="145" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="147"/>
-    </row>
-    <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="145" t="s">
+    </row>
+    <row r="12" ht="14.25" customHeight="1">
+      <c r="A12" s="145" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="145" t="s">
+    <row r="13" ht="14.25" customHeight="1">
+      <c r="A13" s="148" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="13" ht="14.25" customHeight="1">
-      <c r="A13" s="148" t="s">
+      <c r="B13" s="146" t="s">
         <v>82</v>
       </c>
-      <c r="B13" s="146" t="s">
+    </row>
+    <row r="14" ht="14.25" customHeight="1">
+      <c r="A14" s="53" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="53" t="s">
+    <row r="15" ht="14.25" customHeight="1">
+      <c r="A15" s="145" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="145" t="s">
+    <row r="16" ht="14.25" customHeight="1">
+      <c r="A16" s="145" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="145" t="s">
+    <row r="17" ht="14.25" customHeight="1">
+      <c r="A17" s="145" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="145" t="s">
+    <row r="18" ht="14.25" customHeight="1">
+      <c r="A18" s="145" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="18" ht="14.25" customHeight="1">
-      <c r="A18" s="145" t="s">
+    <row r="19" ht="14.25" customHeight="1">
+      <c r="A19" s="145" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="19" ht="14.25" customHeight="1">
-      <c r="A19" s="145" t="s">
+    <row r="20" ht="14.25" customHeight="1">
+      <c r="A20" s="145" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="20" ht="14.25" customHeight="1">
-      <c r="A20" s="145" t="s">
+    <row r="21" ht="14.25" customHeight="1">
+      <c r="A21" s="145" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="21" ht="14.25" customHeight="1">
-      <c r="A21" s="145" t="s">
+    <row r="22" ht="14.25" customHeight="1">
+      <c r="A22" s="145" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="22" ht="14.25" customHeight="1">
-      <c r="A22" s="145" t="s">
+    <row r="23" ht="14.25" customHeight="1">
+      <c r="A23" s="53" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="23" ht="14.25" customHeight="1">
-      <c r="A23" s="53" t="s">
+    <row r="24" ht="14.25" customHeight="1">
+      <c r="A24" s="145" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" s="145" t="s">
+    <row r="25" ht="14.25" customHeight="1">
+      <c r="A25" s="145" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="25" ht="14.25" customHeight="1">
-      <c r="A25" s="145" t="s">
+    <row r="26" ht="14.25" customHeight="1">
+      <c r="A26" s="145" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="26" ht="14.25" customHeight="1">
-      <c r="A26" s="145" t="s">
+    <row r="27" ht="14.25" customHeight="1">
+      <c r="A27" s="145" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="27" ht="14.25" customHeight="1">
-      <c r="A27" s="145" t="s">
+    <row r="28" ht="14.25" customHeight="1">
+      <c r="A28" s="145" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="28" ht="14.25" customHeight="1">
-      <c r="A28" s="145" t="s">
+    <row r="29" ht="14.25" customHeight="1">
+      <c r="A29" s="145" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="29" ht="14.25" customHeight="1">
-      <c r="A29" s="145" t="s">
+    <row r="30" ht="14.25" customHeight="1">
+      <c r="A30" s="145" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="30" ht="14.25" customHeight="1">
-      <c r="A30" s="145" t="s">
+    <row r="31" ht="14.25" customHeight="1">
+      <c r="A31" s="145" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="31" ht="14.25" customHeight="1">
-      <c r="A31" s="145" t="s">
+    <row r="32" ht="14.25" customHeight="1">
+      <c r="A32" s="145" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="32" ht="14.25" customHeight="1">
-      <c r="A32" s="145" t="s">
+    <row r="33" ht="14.25" customHeight="1">
+      <c r="A33" s="145" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="33" ht="14.25" customHeight="1">
-      <c r="A33" s="145" t="s">
+    <row r="34" ht="14.25" customHeight="1">
+      <c r="A34" s="53" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="34" ht="14.25" customHeight="1">
-      <c r="A34" s="53" t="s">
+    <row r="35" ht="14.25" customHeight="1">
+      <c r="A35" s="145" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="35" ht="14.25" customHeight="1">
-      <c r="A35" s="145" t="s">
+    <row r="36" ht="14.25" customHeight="1">
+      <c r="A36" s="53" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="36" ht="14.25" customHeight="1">
-      <c r="A36" s="53" t="s">
+    <row r="37" ht="14.25" customHeight="1">
+      <c r="A37" s="53" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="37" ht="14.25" customHeight="1">
-      <c r="A37" s="53" t="s">
+    <row r="38" ht="14.25" customHeight="1">
+      <c r="A38" s="145" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="38" ht="14.25" customHeight="1">
-      <c r="A38" s="145" t="s">
+    <row r="39" ht="14.25" customHeight="1">
+      <c r="A39" s="145" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="39" ht="14.25" customHeight="1">
-      <c r="A39" s="145" t="s">
+    <row r="40" ht="14.25" customHeight="1">
+      <c r="A40" s="148" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="40" ht="14.25" customHeight="1">
-      <c r="A40" s="148" t="s">
+      <c r="B40" s="146" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" ht="14.25" customHeight="1">
+      <c r="A41" s="145" t="s">
         <v>110</v>
       </c>
-      <c r="B40" s="146" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="41" ht="14.25" customHeight="1">
-      <c r="A41" s="145" t="s">
+    </row>
+    <row r="42" ht="14.25" customHeight="1">
+      <c r="A42" s="148" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="42" ht="14.25" customHeight="1">
-      <c r="A42" s="148" t="s">
+    <row r="43" ht="14.25" customHeight="1">
+      <c r="A43" s="145" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="43" ht="14.25" customHeight="1">
-      <c r="A43" s="145" t="s">
+      <c r="B43" s="146" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="44" ht="14.25" customHeight="1">
+      <c r="A44" s="145" t="s">
         <v>113</v>
       </c>
-      <c r="B43" s="146" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="44" ht="14.25" customHeight="1">
-      <c r="A44" s="145" t="s">
+    </row>
+    <row r="45" ht="14.25" customHeight="1">
+      <c r="A45" s="145" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="45" ht="14.25" customHeight="1">
-      <c r="A45" s="145" t="s">
+      <c r="D45" s="149"/>
+    </row>
+    <row r="46" ht="14.25" customHeight="1">
+      <c r="A46" s="145" t="s">
         <v>115</v>
       </c>
-      <c r="D45" s="149"/>
-    </row>
-    <row r="46" ht="14.25" customHeight="1">
-      <c r="A46" s="145" t="s">
+    </row>
+    <row r="47" ht="14.25" customHeight="1">
+      <c r="A47" s="145" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="47" ht="14.25" customHeight="1">
-      <c r="A47" s="145" t="s">
+    <row r="48" ht="14.25" customHeight="1">
+      <c r="A48" s="145" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="48" ht="14.25" customHeight="1">
-      <c r="A48" s="145" t="s">
+    <row r="49" ht="14.25" customHeight="1">
+      <c r="A49" s="150" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="49" ht="14.25" customHeight="1">
-      <c r="A49" s="150" t="s">
+    <row r="50" ht="14.25" customHeight="1">
+      <c r="A50" s="150" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="50" ht="14.25" customHeight="1">
-      <c r="A50" s="150" t="s">
-        <v>120</v>
-      </c>
-    </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="150" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="52" ht="14.25" customHeight="1"/>

</xml_diff>